<commit_message>
Mudança nos títulos das colunas para evitar erros
</commit_message>
<xml_diff>
--- a/Dados_turma.xlsx
+++ b/Dados_turma.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,24 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
-  <si>
-    <t xml:space="preserve">Código</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="65">
+  <si>
+    <t xml:space="preserve">Cod</t>
   </si>
   <si>
     <t xml:space="preserve">Disciplina</t>
   </si>
   <si>
-    <t xml:space="preserve">Ano e período</t>
+    <t xml:space="preserve">Ano</t>
   </si>
   <si>
     <t xml:space="preserve">Professor</t>
   </si>
   <si>
-    <t xml:space="preserve">Avaliação professor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Média turma</t>
+    <t xml:space="preserve">Av Professor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Med turma</t>
   </si>
   <si>
     <t xml:space="preserve">AP</t>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">Eletromagnetismo I</t>
   </si>
   <si>
+    <t xml:space="preserve">2020/8</t>
+  </si>
+  <si>
     <t xml:space="preserve">Professor1</t>
   </si>
   <si>
@@ -70,6 +73,9 @@
     <t xml:space="preserve">Física III</t>
   </si>
   <si>
+    <t xml:space="preserve">2019/2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Professor3</t>
   </si>
   <si>
@@ -79,6 +85,9 @@
     <t xml:space="preserve">Mecânica clássica I</t>
   </si>
   <si>
+    <t xml:space="preserve">2021/3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Professor4</t>
   </si>
   <si>
@@ -88,9 +97,15 @@
     <t xml:space="preserve">Termodinâmica</t>
   </si>
   <si>
+    <t xml:space="preserve">2018/7</t>
+  </si>
+  <si>
     <t xml:space="preserve">Professor5</t>
   </si>
   <si>
+    <t xml:space="preserve">2018/3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Professor2</t>
   </si>
   <si>
@@ -100,9 +115,15 @@
     <t xml:space="preserve">Física I</t>
   </si>
   <si>
+    <t xml:space="preserve">2020/2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Professor6</t>
   </si>
   <si>
+    <t xml:space="preserve">2022/8</t>
+  </si>
+  <si>
     <t xml:space="preserve">IFI0161</t>
   </si>
   <si>
@@ -115,6 +136,9 @@
     <t xml:space="preserve">Física experimental II</t>
   </si>
   <si>
+    <t xml:space="preserve">2017/7</t>
+  </si>
+  <si>
     <t xml:space="preserve">IFI0254</t>
   </si>
   <si>
@@ -127,6 +151,9 @@
     <t xml:space="preserve">Eletromagnetismo II</t>
   </si>
   <si>
+    <t xml:space="preserve">2022/3</t>
+  </si>
+  <si>
     <t xml:space="preserve">IFI0506</t>
   </si>
   <si>
@@ -139,12 +166,18 @@
     <t xml:space="preserve">Física experimental I</t>
   </si>
   <si>
+    <t xml:space="preserve">2023/2</t>
+  </si>
+  <si>
     <t xml:space="preserve">IFI0093</t>
   </si>
   <si>
     <t xml:space="preserve">Física IV</t>
   </si>
   <si>
+    <t xml:space="preserve">2016/7</t>
+  </si>
+  <si>
     <t xml:space="preserve">IFI0245</t>
   </si>
   <si>
@@ -154,12 +187,21 @@
     <t xml:space="preserve">Professor7</t>
   </si>
   <si>
+    <t xml:space="preserve">2019/8</t>
+  </si>
+  <si>
     <t xml:space="preserve">IFI0441</t>
   </si>
   <si>
     <t xml:space="preserve">Física experimental IV</t>
   </si>
   <si>
+    <t xml:space="preserve">2017/8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/7</t>
+  </si>
+  <si>
     <t xml:space="preserve">IFI0627</t>
   </si>
   <si>
@@ -170,15 +212,20 @@
   </si>
   <si>
     <t xml:space="preserve">Mecânica clássica II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017/2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$-409]mm/dd/yy"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[$-409]General"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -265,7 +312,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -294,6 +341,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -306,6 +361,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -314,7 +475,7 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L21" activeCellId="0" sqref="L21"/>
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -377,13 +538,13 @@
       <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="5" t="n">
-        <v>2020.2</v>
+      <c r="C2" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="E2" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>2.64354037337927</v>
       </c>
@@ -414,18 +575,18 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>2019.1</v>
+        <v>16</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>3.83381772538097</v>
       </c>
@@ -456,18 +617,18 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>2021.1</v>
+        <v>20</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="E4" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>4.65688679578195</v>
       </c>
@@ -502,18 +663,18 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>2018.2</v>
+        <v>24</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="E5" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>0.181907328880617</v>
       </c>
@@ -548,18 +709,18 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>2018.1</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="6" t="n">
+        <v>28</v>
+      </c>
+      <c r="E6" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>5.9756290433757</v>
       </c>
@@ -594,18 +755,18 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>2020.1</v>
+        <v>30</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="E7" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>5.13134269112446</v>
       </c>
@@ -645,13 +806,13 @@
       <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5" t="n">
-        <v>2022.2</v>
+      <c r="C8" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="E8" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>9.26758513213467</v>
       </c>
@@ -686,18 +847,18 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>2019.1</v>
+        <v>35</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="E9" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>0.327128278474887</v>
       </c>
@@ -732,18 +893,18 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="5" t="n">
-        <v>2017.2</v>
+        <v>37</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="E10" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>5.76686052258093</v>
       </c>
@@ -778,18 +939,18 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="5" t="n">
-        <v>2021.2</v>
+        <v>40</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="6" t="n">
+        <v>28</v>
+      </c>
+      <c r="E11" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>0.429853771178466</v>
       </c>
@@ -824,18 +985,18 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="5" t="n">
-        <v>2022.1</v>
+        <v>42</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="E12" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>5.83932737880585</v>
       </c>
@@ -870,18 +1031,18 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="5" t="n">
-        <v>2020.2</v>
+        <v>24</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="E13" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>7.25867658002676</v>
       </c>
@@ -916,18 +1077,18 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="5" t="n">
-        <v>2018.2</v>
+        <v>45</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="6" t="n">
+        <v>28</v>
+      </c>
+      <c r="E14" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>7.48442841818645</v>
       </c>
@@ -962,18 +1123,18 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="5" t="n">
-        <v>2019.1</v>
+        <v>47</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="E15" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>5.33553480948134</v>
       </c>
@@ -1008,18 +1169,18 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="5" t="n">
-        <v>2023.1</v>
+        <v>20</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="E16" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>3.26863925676879</v>
       </c>
@@ -1054,18 +1215,18 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="5" t="n">
-        <v>2016.2</v>
+        <v>50</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="E17" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>7.62605078784932</v>
       </c>
@@ -1100,18 +1261,18 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="5" t="n">
-        <v>2021.1</v>
+        <v>53</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="6" t="n">
+        <v>54</v>
+      </c>
+      <c r="E18" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>3.37869428267789</v>
       </c>
@@ -1146,18 +1307,18 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="5" t="n">
-        <v>2022.1</v>
+        <v>30</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="E19" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>2.38570419946135</v>
       </c>
@@ -1197,13 +1358,13 @@
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="5" t="n">
-        <v>2019.2</v>
+      <c r="C20" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="6" t="n">
+        <v>28</v>
+      </c>
+      <c r="E20" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>4.74243014035344</v>
       </c>
@@ -1238,18 +1399,18 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="5" t="n">
-        <v>2021.1</v>
+        <v>57</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="6" t="n">
+        <v>54</v>
+      </c>
+      <c r="E21" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>4.02785762089647</v>
       </c>
@@ -1284,18 +1445,18 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="5" t="n">
-        <v>2017.2</v>
+        <v>45</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="E22" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>2.7692290888171</v>
       </c>
@@ -1330,18 +1491,18 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="5" t="n">
-        <v>2023.2</v>
+        <v>40</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="E23" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>2.36024349629491</v>
       </c>
@@ -1376,18 +1537,18 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="5" t="n">
-        <v>2016.2</v>
+        <v>61</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="6" t="n">
+        <v>28</v>
+      </c>
+      <c r="E24" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>0.358389981548741</v>
       </c>
@@ -1422,18 +1583,18 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="5" t="n">
-        <v>2022.1</v>
+        <v>35</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="E25" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>7.66590989788858</v>
       </c>
@@ -1468,18 +1629,18 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="5" t="n">
-        <v>2018.2</v>
+        <v>63</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="E26" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>4.78726800246078</v>
       </c>
@@ -1514,18 +1675,18 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="5" t="n">
-        <v>2017.1</v>
+        <v>57</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="6" t="n">
+        <v>54</v>
+      </c>
+      <c r="E27" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>5.87167738995207</v>
       </c>
@@ -1560,18 +1721,18 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="5" t="n">
-        <v>2019.1</v>
+        <v>42</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="E28" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>8.41397299759646</v>
       </c>
@@ -1606,18 +1767,18 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="5" t="n">
-        <v>2021.1</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="6" t="n">
+      <c r="E29" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>3.02393657031875</v>
       </c>
@@ -1652,18 +1813,18 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="5" t="n">
-        <v>2022.1</v>
+        <v>53</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="E30" s="7" t="n">
         <f aca="false">_xlfn.ORG.LIBREOFFICE.RAND.NV()*10</f>
         <v>0.834788732097054</v>
       </c>

</xml_diff>

<commit_message>
Mudando o nome da coluna novamente
</commit_message>
<xml_diff>
--- a/Dados_turma.xlsx
+++ b/Dados_turma.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Disciplina</t>
   </si>
   <si>
-    <t xml:space="preserve">Ano</t>
+    <t xml:space="preserve">Turma</t>
   </si>
   <si>
     <t xml:space="preserve">Professor</t>
@@ -221,11 +221,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$-409]mm/dd/yy"/>
+    <numFmt numFmtId="165" formatCode="[$-409]yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="[$-409]General"/>
+    <numFmt numFmtId="167" formatCode="[$-409]yy/mm/dd"/>
+    <numFmt numFmtId="168" formatCode="[$-409]General"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -312,7 +313,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -346,6 +347,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -475,7 +480,7 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -622,7 +627,7 @@
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -668,7 +673,7 @@
       <c r="B5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -714,7 +719,7 @@
       <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -760,7 +765,7 @@
       <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>31</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -806,7 +811,7 @@
       <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -852,7 +857,7 @@
       <c r="B9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -898,7 +903,7 @@
       <c r="B10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -944,7 +949,7 @@
       <c r="B11" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -990,7 +995,7 @@
       <c r="B12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -1036,7 +1041,7 @@
       <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -1082,7 +1087,7 @@
       <c r="B14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1128,7 +1133,7 @@
       <c r="B15" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -1174,7 +1179,7 @@
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="9" t="s">
         <v>48</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -1220,7 +1225,7 @@
       <c r="B17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>51</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -1266,7 +1271,7 @@
       <c r="B18" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -1312,7 +1317,7 @@
       <c r="B19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -1358,7 +1363,7 @@
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="9" t="s">
         <v>55</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -1404,7 +1409,7 @@
       <c r="B21" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -1450,7 +1455,7 @@
       <c r="B22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="9" t="s">
         <v>58</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -1496,7 +1501,7 @@
       <c r="B23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="9" t="s">
         <v>59</v>
       </c>
       <c r="D23" s="5" t="s">
@@ -1542,7 +1547,7 @@
       <c r="B24" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="9" t="s">
         <v>51</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -1588,7 +1593,7 @@
       <c r="B25" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D25" s="5" t="s">
@@ -1634,7 +1639,7 @@
       <c r="B26" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D26" s="5" t="s">
@@ -1680,7 +1685,7 @@
       <c r="B27" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="9" t="s">
         <v>64</v>
       </c>
       <c r="D27" s="5" t="s">
@@ -1726,7 +1731,7 @@
       <c r="B28" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="5" t="s">
@@ -1772,7 +1777,7 @@
       <c r="B29" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D29" s="5" t="s">
@@ -1818,7 +1823,7 @@
       <c r="B30" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D30" s="5" t="s">

</xml_diff>

<commit_message>
Aplicando as mesmas mudanças da branch Google-sheets
</commit_message>
<xml_diff>
--- a/Dados_turma.xlsx
+++ b/Dados_turma.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="65">
   <si>
-    <t xml:space="preserve">Cod</t>
+    <t xml:space="preserve">Código</t>
   </si>
   <si>
     <t xml:space="preserve">Disciplina</t>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Av Professor</t>
   </si>
   <si>
-    <t xml:space="preserve">Med turma</t>
+    <t xml:space="preserve">Média turma</t>
   </si>
   <si>
     <t xml:space="preserve">AP</t>
@@ -480,7 +480,7 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>